<commit_message>
report update and results version 1
</commit_message>
<xml_diff>
--- a/Analysis Result.xlsx
+++ b/Analysis Result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>1. Bytecode</t>
   </si>
@@ -60,6 +60,227 @@
   </si>
   <si>
     <t>3. Solidity code</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1. Bytecode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2. Bytecode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3. Bytecode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4. Bytecode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5. Bytecode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <t>Mythril identified Re-entrancy vulnerabilities with the similar analysis report as in the case for solidity code analysis. The Bytecode analysis was not applicable with the context of Slither</t>
+  </si>
+  <si>
+    <t>Mythril could not identify Unchecked Enternal call vulnerability as in the case for solidity code analysis. The Bytecode analysis was not applicable with the context of Slither</t>
+  </si>
+  <si>
+    <t>Manual analysis could not find vulnerabilities in the bytecode.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2. EVM Opcode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3. EVM Opcode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4. EVM Opcode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5. EVM Opcode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6. EVM Opcode Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <t>Mythril and Slither are does not support to detect any vulnerabilities through the EVM opcode analysis.</t>
+  </si>
+  <si>
+    <t>Manual analysis identified re entrancy vulnerability through aforementioned dissemination of opcodes.</t>
+  </si>
+  <si>
+    <t>Manual analysis identified Unchecked Enternal call vulnerability through aforementioned dissemination of opcodes.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3. Solidity Code Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4. Solidity Code Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5. Solidity Code Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6. Solidity Code Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7. Solidity Code Analysis:</t>
+    </r>
+  </si>
+  <si>
+    <t>Both Mythril and Slither identified re-entrancy vulnerability during Solidity code analysis.</t>
+  </si>
+  <si>
+    <t>Both Mythril and Slither identified Unchecked Enternal call vulnerability during Solidity code analysis.</t>
+  </si>
+  <si>
+    <t>Manual analysis also identified re-entrancy vulnerability and an attempt with the updated code was provided.</t>
+  </si>
+  <si>
+    <t>Manual analysis also identified Unchecked Enternal call vulnerability and an attempt with the updated code was provided.</t>
   </si>
   <si>
     <t>0 PUSH1 0x80</t>
@@ -210,7 +431,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +466,19 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -711,137 +945,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,6 +1089,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1460,17 +1700,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:F23"/>
+  <dimension ref="A3:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="24.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="49.3809523809524" customWidth="1"/>
+    <col min="3" max="3" width="59.7809523809524" customWidth="1"/>
     <col min="4" max="4" width="18.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
@@ -1750,6 +1990,193 @@
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" spans="2:6">
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" spans="2:6">
+      <c r="B26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="2:6">
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" spans="2:6">
+      <c r="B28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" spans="2:6">
+      <c r="B29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" spans="2:6">
+      <c r="B30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" spans="2:6">
+      <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" spans="2:6">
+      <c r="B32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" spans="2:6">
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" spans="2:6">
+      <c r="B34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" spans="2:6">
+      <c r="B35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1780,186 +2207,186 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>